<commit_message>
Plying with the ammonia script, nothing major
</commit_message>
<xml_diff>
--- a/dataframes/experimental_data_density/0357.xlsx
+++ b/dataframes/experimental_data_density/0357.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/cd318_ic_ac_uk/Documents/UNI/PhD/Code/GitHub repos/EOS/dataframes/experimental_data_density/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{908FB66B-D971-4CD3-BA9D-F63E519B3F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2649DE76-6D5B-4BCD-8964-BA88D60EDA67}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{908FB66B-D971-4CD3-BA9D-F63E519B3F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13AEC012-3335-43C0-80EF-954A1DF72435}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE2EAF4-2088-492C-959D-3D95DA367FD4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE2EAF4-2088-492C-959D-3D95DA367FD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,6 +115,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,7 +441,7 @@
   <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,16 +501,16 @@
         <v>10.526315789473685</v>
       </c>
       <c r="G2">
-        <f>0.01*101325/D2*100</f>
-        <v>3.379520108144643E-2</v>
+        <f>0.015*101325/D2*100</f>
+        <v>5.0692801622169652E-2</v>
       </c>
       <c r="H2">
-        <f>0.001/E2*100</f>
-        <v>1.6718214494691969E-4</v>
+        <f>0.001/B2*100</f>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I2">
-        <f>0.5*0.000000001*F2/(9*0.001)</f>
-        <v>5.8479532163742688E-7</v>
+        <f>(0.2/9000+F2/(9*0.001)*0.5*0.000000001)*100</f>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -532,16 +536,16 @@
         <v>11.111111111111112</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="3">0.01*101325/D3*100</f>
-        <v>3.2030749519538756E-2</v>
+        <f t="shared" ref="G3:G66" si="3">0.015*101325/D3*100</f>
+        <v>4.8046124279308142E-2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="4">0.001/E3*100</f>
-        <v>1.6718214494691969E-4</v>
+        <f t="shared" ref="H3:H66" si="4">0.001/B3*100</f>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="5">0.5*0.000000001*F3/(9*0.001)</f>
-        <v>6.1728395061728406E-7</v>
+        <f t="shared" ref="I3:I66" si="5">(0.2/9000+F3/(9*0.001)*0.5*0.000000001)*100</f>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -568,15 +572,15 @@
       </c>
       <c r="G4">
         <f t="shared" si="3"/>
-        <v>2.8538812785388126E-2</v>
+        <v>4.2808219178082189E-2</v>
       </c>
       <c r="H4">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I4">
         <f t="shared" si="5"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -603,15 +607,15 @@
       </c>
       <c r="G5">
         <f t="shared" si="3"/>
-        <v>2.5062656641604009E-2</v>
+        <v>3.759398496240602E-2</v>
       </c>
       <c r="H5">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I5">
         <f t="shared" si="5"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -638,15 +642,15 @@
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>2.1579628830384119E-2</v>
+        <v>3.2369443245576175E-2</v>
       </c>
       <c r="H6">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I6">
         <f t="shared" si="5"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -673,15 +677,15 @@
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
-        <v>1.8102824040550324E-2</v>
+        <v>2.7154236060825489E-2</v>
       </c>
       <c r="H7">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -708,15 +712,15 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>1.6363933889707083E-2</v>
+        <v>2.4545900834560628E-2</v>
       </c>
       <c r="H8">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I8">
         <f t="shared" si="5"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -743,15 +747,15 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>1.4628437682855471E-2</v>
+        <v>2.1942656524283205E-2</v>
       </c>
       <c r="H9">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I9">
         <f t="shared" si="5"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -778,15 +782,15 @@
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>1.288825879623663E-2</v>
+        <v>1.9332388194354944E-2</v>
       </c>
       <c r="H10">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I10">
         <f t="shared" si="5"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -813,15 +817,15 @@
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>1.1149514996097671E-2</v>
+        <v>1.6724272494146503E-2</v>
       </c>
       <c r="H11">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I11">
         <f t="shared" si="5"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -848,15 +852,15 @@
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>9.4117647058823539E-3</v>
+        <v>1.4117647058823528E-2</v>
       </c>
       <c r="H12">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I12">
         <f t="shared" si="5"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -883,15 +887,15 @@
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>7.6687116564417186E-3</v>
+        <v>1.1503067484662576E-2</v>
       </c>
       <c r="H13">
         <f t="shared" si="4"/>
-        <v>1.6718214494691969E-4</v>
+        <v>3.076923076923077E-4</v>
       </c>
       <c r="I13">
         <f t="shared" si="5"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -918,15 +922,15 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>3.5348179568752212E-2</v>
+        <v>5.3022269353128322E-2</v>
       </c>
       <c r="H14">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I14">
         <f t="shared" si="5"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -953,15 +957,15 @@
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>3.351206434316354E-2</v>
+        <v>5.0268096514745307E-2</v>
       </c>
       <c r="H15">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I15">
         <f t="shared" si="5"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -988,15 +992,15 @@
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>2.9895366218236172E-2</v>
+        <v>4.4843049327354258E-2</v>
       </c>
       <c r="H16">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I16">
         <f t="shared" si="5"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1023,15 +1027,15 @@
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>2.6260504201680673E-2</v>
+        <v>3.9390756302521007E-2</v>
       </c>
       <c r="H17">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I17">
         <f t="shared" si="5"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1058,15 +1062,15 @@
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
-        <v>2.2634676324128564E-2</v>
+        <v>3.3952014486192852E-2</v>
       </c>
       <c r="H18">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I18">
         <f t="shared" si="5"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1093,15 +1097,15 @@
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>1.9004180919802355E-2</v>
+        <v>2.8506271379703536E-2</v>
       </c>
       <c r="H19">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I19">
         <f t="shared" si="5"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1128,15 +1132,15 @@
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>1.7193947730398899E-2</v>
+        <v>2.5790921595598346E-2</v>
       </c>
       <c r="H20">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I20">
         <f t="shared" si="5"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1163,15 +1167,15 @@
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>1.5377518068583732E-2</v>
+        <v>2.3066277102875593E-2</v>
       </c>
       <c r="H21">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I21">
         <f t="shared" si="5"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1198,15 +1202,15 @@
       </c>
       <c r="G22">
         <f t="shared" si="3"/>
-        <v>1.3572204125950052E-2</v>
+        <v>2.035830618892508E-2</v>
       </c>
       <c r="H22">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I22">
         <f t="shared" si="5"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1233,15 +1237,15 @@
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
-        <v>1.175226231049477E-2</v>
+        <v>1.7628393465742156E-2</v>
       </c>
       <c r="H23">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I23">
         <f t="shared" si="5"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1268,15 +1272,15 @@
       </c>
       <c r="G24">
         <f t="shared" si="3"/>
-        <v>9.9393698439518945E-3</v>
+        <v>1.4909054765927842E-2</v>
       </c>
       <c r="H24">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I24">
         <f t="shared" si="5"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1303,15 +1307,15 @@
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>8.1234768480909821E-3</v>
+        <v>1.2185215272136474E-2</v>
       </c>
       <c r="H25">
         <f t="shared" si="4"/>
-        <v>1.7447439588240429E-4</v>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="I25">
         <f t="shared" si="5"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1338,15 +1342,15 @@
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>3.7064492216456635E-2</v>
+        <v>5.5596738324684952E-2</v>
       </c>
       <c r="H26">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I26">
         <f t="shared" si="5"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1373,15 +1377,15 @@
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
-        <v>3.5161744022503515E-2</v>
+        <v>5.2742616033755269E-2</v>
       </c>
       <c r="H27">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I27">
         <f t="shared" si="5"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1408,15 +1412,15 @@
       </c>
       <c r="G28">
         <f t="shared" si="3"/>
-        <v>3.1377470975839344E-2</v>
+        <v>4.7066206463759024E-2</v>
       </c>
       <c r="H28">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I28">
         <f t="shared" si="5"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1443,15 +1447,15 @@
       </c>
       <c r="G29">
         <f t="shared" si="3"/>
-        <v>2.7586206896551724E-2</v>
+        <v>4.1379310344827586E-2</v>
       </c>
       <c r="H29">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I29">
         <f t="shared" si="5"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1478,15 +1482,15 @@
       </c>
       <c r="G30">
         <f t="shared" si="3"/>
-        <v>2.3809523809523808E-2</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="H30">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I30">
         <f t="shared" si="5"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1513,15 +1517,15 @@
       </c>
       <c r="G31">
         <f t="shared" si="3"/>
-        <v>2.0016012810248198E-2</v>
+        <v>3.0024019215372295E-2</v>
       </c>
       <c r="H31">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I31">
         <f t="shared" si="5"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1548,15 +1552,15 @@
       </c>
       <c r="G32">
         <f t="shared" si="3"/>
-        <v>1.8122508155128669E-2</v>
+        <v>2.7183762232693004E-2</v>
       </c>
       <c r="H32">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I32">
         <f t="shared" si="5"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1583,15 +1587,15 @@
       </c>
       <c r="G33">
         <f t="shared" si="3"/>
-        <v>1.6228497241155469E-2</v>
+        <v>2.4342745861733205E-2</v>
       </c>
       <c r="H33">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I33">
         <f t="shared" si="5"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1618,15 +1622,15 @@
       </c>
       <c r="G34">
         <f t="shared" si="3"/>
-        <v>1.4332807797047441E-2</v>
+        <v>2.149921169557116E-2</v>
       </c>
       <c r="H34">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I34">
         <f t="shared" si="5"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1653,15 +1657,15 @@
       </c>
       <c r="G35">
         <f t="shared" si="3"/>
-        <v>1.2430080795525171E-2</v>
+        <v>1.8645121193287758E-2</v>
       </c>
       <c r="H35">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I35">
         <f t="shared" si="5"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1688,15 +1692,15 @@
       </c>
       <c r="G36">
         <f t="shared" si="3"/>
-        <v>1.0539629005059021E-2</v>
+        <v>1.5809443507588533E-2</v>
       </c>
       <c r="H36">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I36">
         <f t="shared" si="5"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1723,15 +1727,15 @@
       </c>
       <c r="G37">
         <f t="shared" si="3"/>
-        <v>8.6452839975793196E-3</v>
+        <v>1.2967925996368982E-2</v>
       </c>
       <c r="H37">
         <f t="shared" si="4"/>
-        <v>1.8243181610872936E-4</v>
+        <v>3.6363636363636367E-4</v>
       </c>
       <c r="I37">
         <f t="shared" si="5"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1758,15 +1762,15 @@
       </c>
       <c r="G38">
         <f t="shared" si="3"/>
-        <v>3.9001560062402497E-2</v>
+        <v>5.850234009360375E-2</v>
       </c>
       <c r="H38">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I38">
         <f t="shared" si="5"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1793,15 +1797,15 @@
       </c>
       <c r="G39">
         <f t="shared" si="3"/>
-        <v>3.7023324694557574E-2</v>
+        <v>5.5534987041836362E-2</v>
       </c>
       <c r="H39">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I39">
         <f t="shared" si="5"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1828,15 +1832,15 @@
       </c>
       <c r="G40">
         <f t="shared" si="3"/>
-        <v>3.3036009250082585E-2</v>
+        <v>4.9554013875123884E-2</v>
       </c>
       <c r="H40">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I40">
         <f t="shared" si="5"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1863,15 +1867,15 @@
       </c>
       <c r="G41">
         <f t="shared" si="3"/>
-        <v>2.9078220412910728E-2</v>
+        <v>4.3617330619366096E-2</v>
       </c>
       <c r="H41">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I41">
         <f t="shared" si="5"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1898,15 +1902,15 @@
       </c>
       <c r="G42">
         <f t="shared" si="3"/>
-        <v>2.5106703489831784E-2</v>
+        <v>3.7660055234747677E-2</v>
       </c>
       <c r="H42">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I42">
         <f t="shared" si="5"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1933,15 +1937,15 @@
       </c>
       <c r="G43">
         <f t="shared" si="3"/>
-        <v>2.1128248468201986E-2</v>
+        <v>3.1692372702302976E-2</v>
       </c>
       <c r="H43">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I43">
         <f t="shared" si="5"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1968,15 +1972,15 @@
       </c>
       <c r="G44">
         <f t="shared" si="3"/>
-        <v>1.9149751053236307E-2</v>
+        <v>2.8724626579854463E-2</v>
       </c>
       <c r="H44">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I44">
         <f t="shared" si="5"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2003,15 +2007,15 @@
       </c>
       <c r="G45">
         <f t="shared" si="3"/>
-        <v>1.7164435290078956E-2</v>
+        <v>2.5746652935118432E-2</v>
       </c>
       <c r="H45">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I45">
         <f t="shared" si="5"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2038,15 +2042,15 @@
       </c>
       <c r="G46">
         <f t="shared" si="3"/>
-        <v>1.518372304889159E-2</v>
+        <v>2.2775584573337383E-2</v>
       </c>
       <c r="H46">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I46">
         <f t="shared" si="5"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2073,15 +2077,15 @@
       </c>
       <c r="G47">
         <f t="shared" si="3"/>
-        <v>1.3203063110641672E-2</v>
+        <v>1.9804594665962506E-2</v>
       </c>
       <c r="H47">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I47">
         <f t="shared" si="5"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2108,15 +2112,15 @@
       </c>
       <c r="G48">
         <f t="shared" si="3"/>
-        <v>1.1222085063404781E-2</v>
+        <v>1.6833127595107168E-2</v>
       </c>
       <c r="H48">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I48">
         <f t="shared" si="5"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2143,15 +2147,15 @@
       </c>
       <c r="G49">
         <f t="shared" si="3"/>
-        <v>9.2438528378628211E-3</v>
+        <v>1.3865779256794233E-2</v>
       </c>
       <c r="H49">
         <f t="shared" si="4"/>
-        <v>1.9114976584153686E-4</v>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="I49">
         <f t="shared" si="5"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2178,15 +2182,15 @@
       </c>
       <c r="G50">
         <f t="shared" si="3"/>
-        <v>4.1152263374485597E-2</v>
+        <v>6.1728395061728392E-2</v>
       </c>
       <c r="H50">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I50">
         <f t="shared" si="5"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2213,15 +2217,15 @@
       </c>
       <c r="G51">
         <f t="shared" si="3"/>
-        <v>3.9077764751856196E-2</v>
+        <v>5.8616647127784284E-2</v>
       </c>
       <c r="H51">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I51">
         <f t="shared" si="5"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2248,15 +2252,15 @@
       </c>
       <c r="G52">
         <f t="shared" si="3"/>
-        <v>3.4916201117318434E-2</v>
+        <v>5.2374301675977654E-2</v>
       </c>
       <c r="H52">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I52">
         <f t="shared" si="5"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2283,15 +2287,15 @@
       </c>
       <c r="G53">
         <f t="shared" si="3"/>
-        <v>3.0731407498463426E-2</v>
+        <v>4.6097111247695145E-2</v>
       </c>
       <c r="H53">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I53">
         <f t="shared" si="5"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2318,15 +2322,15 @@
       </c>
       <c r="G54">
         <f t="shared" si="3"/>
-        <v>2.6567481402763018E-2</v>
+        <v>3.9851222104144525E-2</v>
       </c>
       <c r="H54">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I54">
         <f t="shared" si="5"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2353,15 +2357,15 @@
       </c>
       <c r="G55">
         <f t="shared" si="3"/>
-        <v>2.2406453058480841E-2</v>
+        <v>3.3609679587721264E-2</v>
       </c>
       <c r="H55">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I55">
         <f t="shared" si="5"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2388,15 +2392,15 @@
       </c>
       <c r="G56">
         <f t="shared" si="3"/>
-        <v>2.032520325203252E-2</v>
+        <v>3.048780487804878E-2</v>
       </c>
       <c r="H56">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I56">
         <f t="shared" si="5"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2423,15 +2427,15 @@
       </c>
       <c r="G57">
         <f t="shared" si="3"/>
-        <v>1.8244845831052726E-2</v>
+        <v>2.7367268746579094E-2</v>
       </c>
       <c r="H57">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I57">
         <f t="shared" si="5"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2458,15 +2462,15 @@
       </c>
       <c r="G58">
         <f t="shared" si="3"/>
-        <v>1.6168148746968473E-2</v>
+        <v>2.4252223120452707E-2</v>
       </c>
       <c r="H58">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I58">
         <f t="shared" si="5"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2493,15 +2497,15 @@
       </c>
       <c r="G59">
         <f t="shared" si="3"/>
-        <v>1.4090460758066789E-2</v>
+        <v>2.1135691137100183E-2</v>
       </c>
       <c r="H59">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I59">
         <f t="shared" si="5"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2528,15 +2532,15 @@
       </c>
       <c r="G60">
         <f t="shared" si="3"/>
-        <v>1.2017786323759164E-2</v>
+        <v>1.8026679485638745E-2</v>
       </c>
       <c r="H60">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I60">
         <f t="shared" si="5"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2563,15 +2567,15 @@
       </c>
       <c r="G61">
         <f t="shared" si="3"/>
-        <v>9.949258780220873E-3</v>
+        <v>1.4923888170331311E-2</v>
       </c>
       <c r="H61">
         <f t="shared" si="4"/>
-        <v>2.0074274816822245E-4</v>
+        <v>4.4444444444444441E-4</v>
       </c>
       <c r="I61">
         <f t="shared" si="5"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2598,15 +2602,15 @@
       </c>
       <c r="G62">
         <f t="shared" si="3"/>
-        <v>4.3610989969472311E-2</v>
+        <v>6.5416484954208459E-2</v>
       </c>
       <c r="H62">
         <f t="shared" si="4"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I62">
         <f t="shared" si="5"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2633,15 +2637,15 @@
       </c>
       <c r="G63">
         <f t="shared" si="3"/>
-        <v>4.1407867494824016E-2</v>
+        <v>6.2111801242236024E-2</v>
       </c>
       <c r="H63">
         <f t="shared" si="4"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I63">
         <f t="shared" si="5"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2668,15 +2672,15 @@
       </c>
       <c r="G64">
         <f t="shared" si="3"/>
-        <v>3.7023324694557574E-2</v>
+        <v>5.5534987041836362E-2</v>
       </c>
       <c r="H64">
         <f t="shared" si="4"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I64">
         <f t="shared" si="5"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2703,15 +2707,15 @@
       </c>
       <c r="G65">
         <f t="shared" si="3"/>
-        <v>3.2637075718015669E-2</v>
+        <v>4.8955613577023493E-2</v>
       </c>
       <c r="H65">
         <f t="shared" si="4"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I65">
         <f t="shared" si="5"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2738,15 +2742,15 @@
       </c>
       <c r="G66">
         <f t="shared" si="3"/>
-        <v>2.8248587570621469E-2</v>
+        <v>4.2372881355932202E-2</v>
       </c>
       <c r="H66">
         <f t="shared" si="4"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I66">
         <f t="shared" si="5"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2772,16 +2776,16 @@
         <v>20</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G130" si="9">0.01*101325/D67*100</f>
-        <v>2.3872045834328001E-2</v>
+        <f t="shared" ref="G67:G130" si="9">0.015*101325/D67*100</f>
+        <v>3.5808068751492006E-2</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H130" si="10">0.001/E67*100</f>
-        <v>2.1134946634259749E-4</v>
+        <f t="shared" ref="H67:H130" si="10">0.001/B67*100</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I130" si="11">0.5*0.000000001*F67/(9*0.001)</f>
-        <v>1.111111111111111E-6</v>
+        <f t="shared" ref="I67:I130" si="11">(0.2/9000+F67/(9*0.001)*0.5*0.000000001)*100</f>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2808,15 +2812,15 @@
       </c>
       <c r="G68">
         <f t="shared" si="9"/>
-        <v>2.1682567215958369E-2</v>
+        <v>3.2523850823937557E-2</v>
       </c>
       <c r="H68">
         <f t="shared" si="10"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I68">
         <f t="shared" si="11"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2843,15 +2847,15 @@
       </c>
       <c r="G69">
         <f t="shared" si="9"/>
-        <v>1.9496977968414896E-2</v>
+        <v>2.9245466952622347E-2</v>
       </c>
       <c r="H69">
         <f t="shared" si="10"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I69">
         <f t="shared" si="11"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2878,15 +2882,15 @@
       </c>
       <c r="G70">
         <f t="shared" si="9"/>
-        <v>1.7319016279875303E-2</v>
+        <v>2.5978524419812955E-2</v>
       </c>
       <c r="H70">
         <f t="shared" si="10"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I70">
         <f t="shared" si="11"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -2913,15 +2917,15 @@
       </c>
       <c r="G71">
         <f t="shared" si="9"/>
-        <v>1.514004542013626E-2</v>
+        <v>2.2710068130204389E-2</v>
       </c>
       <c r="H71">
         <f t="shared" si="10"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I71">
         <f t="shared" si="11"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2948,15 +2952,15 @@
       </c>
       <c r="G72">
         <f t="shared" si="9"/>
-        <v>1.2965123816932451E-2</v>
+        <v>1.9447685725398678E-2</v>
       </c>
       <c r="H72">
         <f t="shared" si="10"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I72">
         <f t="shared" si="11"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2983,15 +2987,15 @@
       </c>
       <c r="G73">
         <f t="shared" si="9"/>
-        <v>1.0802635843145727E-2</v>
+        <v>1.6203953764718591E-2</v>
       </c>
       <c r="H73">
         <f t="shared" si="10"/>
-        <v>2.1134946634259749E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I73">
         <f t="shared" si="11"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3018,15 +3022,15 @@
       </c>
       <c r="G74">
         <f t="shared" si="9"/>
-        <v>4.63821892393321E-2</v>
+        <v>6.9573283858998136E-2</v>
       </c>
       <c r="H74">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I74">
         <f t="shared" si="11"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3053,15 +3057,15 @@
       </c>
       <c r="G75">
         <f t="shared" si="9"/>
-        <v>4.405286343612335E-2</v>
+        <v>6.6079295154185022E-2</v>
       </c>
       <c r="H75">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I75">
         <f t="shared" si="11"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3088,15 +3092,15 @@
       </c>
       <c r="G76">
         <f t="shared" si="9"/>
-        <v>3.9432176656151417E-2</v>
+        <v>5.9148264984227129E-2</v>
       </c>
       <c r="H76">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I76">
         <f t="shared" si="11"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3123,15 +3127,15 @@
       </c>
       <c r="G77">
         <f t="shared" si="9"/>
-        <v>3.4794711203897009E-2</v>
+        <v>5.2192066805845504E-2</v>
       </c>
       <c r="H77">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I77">
         <f t="shared" si="11"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3158,15 +3162,15 @@
       </c>
       <c r="G78">
         <f t="shared" si="9"/>
-        <v>3.0175015087507546E-2</v>
+        <v>4.5262522631261314E-2</v>
       </c>
       <c r="H78">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I78">
         <f t="shared" si="11"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3193,15 +3197,15 @@
       </c>
       <c r="G79">
         <f t="shared" si="9"/>
-        <v>2.5555839509327882E-2</v>
+        <v>3.8333759263991816E-2</v>
       </c>
       <c r="H79">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I79">
         <f t="shared" si="11"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3228,15 +3232,15 @@
       </c>
       <c r="G80">
         <f t="shared" si="9"/>
-        <v>2.3250406882120437E-2</v>
+        <v>3.4875610323180657E-2</v>
       </c>
       <c r="H80">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I80">
         <f t="shared" si="11"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3263,15 +3267,15 @@
       </c>
       <c r="G81">
         <f t="shared" si="9"/>
-        <v>2.0951183741881416E-2</v>
+        <v>3.1426775612822123E-2</v>
       </c>
       <c r="H81">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I81">
         <f t="shared" si="11"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3298,15 +3302,15 @@
       </c>
       <c r="G82">
         <f t="shared" si="9"/>
-        <v>1.8653236336504384E-2</v>
+        <v>2.7979854504756579E-2</v>
       </c>
       <c r="H82">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I82">
         <f t="shared" si="11"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3333,15 +3337,15 @@
       </c>
       <c r="G83">
         <f t="shared" si="9"/>
-        <v>1.6363933889707083E-2</v>
+        <v>2.4545900834560628E-2</v>
       </c>
       <c r="H83">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I83">
         <f t="shared" si="11"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3368,15 +3372,15 @@
       </c>
       <c r="G84">
         <f t="shared" si="9"/>
-        <v>1.4088475626937165E-2</v>
+        <v>2.1132713440405747E-2</v>
       </c>
       <c r="H84">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I84">
         <f t="shared" si="11"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3403,15 +3407,15 @@
       </c>
       <c r="G85">
         <f t="shared" si="9"/>
-        <v>1.1828720132481665E-2</v>
+        <v>1.7743080198722498E-2</v>
       </c>
       <c r="H85">
         <f t="shared" si="10"/>
-        <v>2.2313957380341404E-4</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="I85">
         <f t="shared" si="11"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3438,15 +3442,15 @@
       </c>
       <c r="G86">
         <f t="shared" si="9"/>
-        <v>4.9554013875123884E-2</v>
+        <v>7.4331020812685833E-2</v>
       </c>
       <c r="H86">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I86">
         <f t="shared" si="11"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3473,15 +3477,15 @@
       </c>
       <c r="G87">
         <f t="shared" si="9"/>
-        <v>4.7103155911446065E-2</v>
+        <v>7.0654733867169098E-2</v>
       </c>
       <c r="H87">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I87">
         <f t="shared" si="11"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3508,15 +3512,15 @@
       </c>
       <c r="G88">
         <f t="shared" si="9"/>
-        <v>4.2194092827004218E-2</v>
+        <v>6.3291139240506333E-2</v>
       </c>
       <c r="H88">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I88">
         <f t="shared" si="11"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3543,15 +3547,15 @@
       </c>
       <c r="G89">
         <f t="shared" si="9"/>
-        <v>3.7299515106303617E-2</v>
+        <v>5.5949272659455422E-2</v>
       </c>
       <c r="H89">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I89">
         <f t="shared" si="11"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3578,15 +3582,15 @@
       </c>
       <c r="G90">
         <f t="shared" si="9"/>
-        <v>3.240440699935191E-2</v>
+        <v>4.8606610499027869E-2</v>
       </c>
       <c r="H90">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I90">
         <f t="shared" si="11"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3613,15 +3617,15 @@
       </c>
       <c r="G91">
         <f t="shared" si="9"/>
-        <v>2.7525461051472612E-2</v>
+        <v>4.1288191577208914E-2</v>
       </c>
       <c r="H91">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I91">
         <f t="shared" si="11"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3648,15 +3652,15 @@
       </c>
       <c r="G92">
         <f t="shared" si="9"/>
-        <v>2.5094102885821829E-2</v>
+        <v>3.7641154328732752E-2</v>
       </c>
       <c r="H92">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I92">
         <f t="shared" si="11"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3683,15 +3687,15 @@
       </c>
       <c r="G93">
         <f t="shared" si="9"/>
-        <v>2.2670596236681023E-2</v>
+        <v>3.4005894355021535E-2</v>
       </c>
       <c r="H93">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I93">
         <f t="shared" si="11"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -3718,15 +3722,15 @@
       </c>
       <c r="G94">
         <f t="shared" si="9"/>
-        <v>2.0259319286871962E-2</v>
+        <v>3.0388978930307946E-2</v>
       </c>
       <c r="H94">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I94">
         <f t="shared" si="11"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3753,15 +3757,15 @@
       </c>
       <c r="G95">
         <f t="shared" si="9"/>
-        <v>1.7853954650955184E-2</v>
+        <v>2.6780931976432779E-2</v>
       </c>
       <c r="H95">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I95">
         <f t="shared" si="11"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3788,15 +3792,15 @@
       </c>
       <c r="G96">
         <f t="shared" si="9"/>
-        <v>1.5467904098994583E-2</v>
+        <v>2.3201856148491878E-2</v>
       </c>
       <c r="H96">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I96">
         <f t="shared" si="11"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3823,15 +3827,15 @@
       </c>
       <c r="G97">
         <f t="shared" si="9"/>
-        <v>1.3116474291710388E-2</v>
+        <v>1.9674711437565585E-2</v>
       </c>
       <c r="H97">
         <f t="shared" si="10"/>
-        <v>2.3632281696797826E-4</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="I97">
         <f t="shared" si="11"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3858,15 +3862,15 @@
       </c>
       <c r="G98">
         <f t="shared" si="9"/>
-        <v>5.3248136315228969E-2</v>
+        <v>7.9872204472843447E-2</v>
       </c>
       <c r="H98">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I98">
         <f t="shared" si="11"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -3893,15 +3897,15 @@
       </c>
       <c r="G99">
         <f t="shared" si="9"/>
-        <v>5.0632911392405069E-2</v>
+        <v>7.5949367088607597E-2</v>
       </c>
       <c r="H99">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I99">
         <f t="shared" si="11"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -3928,15 +3932,15 @@
       </c>
       <c r="G100">
         <f t="shared" si="9"/>
-        <v>4.5454545454545456E-2</v>
+        <v>6.8181818181818191E-2</v>
       </c>
       <c r="H100">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I100">
         <f t="shared" si="11"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -3963,15 +3967,15 @@
       </c>
       <c r="G101">
         <f t="shared" si="9"/>
-        <v>4.0241448692152917E-2</v>
+        <v>6.0362173038229376E-2</v>
       </c>
       <c r="H101">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I101">
         <f t="shared" si="11"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -3998,15 +4002,15 @@
       </c>
       <c r="G102">
         <f t="shared" si="9"/>
-        <v>3.5075412136092596E-2</v>
+        <v>5.2613118204138901E-2</v>
       </c>
       <c r="H102">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I102">
         <f t="shared" si="11"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4033,15 +4037,15 @@
       </c>
       <c r="G103">
         <f t="shared" si="9"/>
-        <v>2.9904306220095694E-2</v>
+        <v>4.4856459330143539E-2</v>
       </c>
       <c r="H103">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I103">
         <f t="shared" si="11"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4068,15 +4072,15 @@
       </c>
       <c r="G104">
         <f t="shared" si="9"/>
-        <v>2.7329871549603715E-2</v>
+        <v>4.0994807324405573E-2</v>
       </c>
       <c r="H104">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I104">
         <f t="shared" si="11"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4103,15 +4107,15 @@
       </c>
       <c r="G105">
         <f t="shared" si="9"/>
-        <v>2.4777006937561942E-2</v>
+        <v>3.7165510406342916E-2</v>
       </c>
       <c r="H105">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I105">
         <f t="shared" si="11"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4138,15 +4142,15 @@
       </c>
       <c r="G106">
         <f t="shared" si="9"/>
-        <v>2.2227161591464768E-2</v>
+        <v>3.3340742387197156E-2</v>
       </c>
       <c r="H106">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I106">
         <f t="shared" si="11"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4173,15 +4177,15 @@
       </c>
       <c r="G107">
         <f t="shared" si="9"/>
-        <v>1.9708316909735908E-2</v>
+        <v>2.9562475364603862E-2</v>
       </c>
       <c r="H107">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I107">
         <f t="shared" si="11"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4208,15 +4212,15 @@
       </c>
       <c r="G108">
         <f t="shared" si="9"/>
-        <v>1.722356183258698E-2</v>
+        <v>2.5835342748880469E-2</v>
       </c>
       <c r="H108">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I108">
         <f t="shared" si="11"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4243,15 +4247,15 @@
       </c>
       <c r="G109">
         <f t="shared" si="9"/>
-        <v>1.4801657785671994E-2</v>
+        <v>2.2202486678507993E-2</v>
       </c>
       <c r="H109">
         <f t="shared" si="10"/>
-        <v>2.5116162250408139E-4</v>
+        <v>7.9999999999999993E-4</v>
       </c>
       <c r="I109">
         <f t="shared" si="11"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4278,15 +4282,15 @@
       </c>
       <c r="G110">
         <f t="shared" si="9"/>
-        <v>5.7603686635944701E-2</v>
+        <v>8.6405529953917051E-2</v>
       </c>
       <c r="H110">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I110">
         <f t="shared" si="11"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4313,15 +4317,15 @@
       </c>
       <c r="G111">
         <f t="shared" si="9"/>
-        <v>5.4824561403508783E-2</v>
+        <v>8.2236842105263164E-2</v>
       </c>
       <c r="H111">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I111">
         <f t="shared" si="11"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4348,15 +4352,15 @@
       </c>
       <c r="G112">
         <f t="shared" si="9"/>
-        <v>4.9309664694280081E-2</v>
+        <v>7.3964497041420121E-2</v>
       </c>
       <c r="H112">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I112">
         <f t="shared" si="11"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4383,15 +4387,15 @@
       </c>
       <c r="G113">
         <f t="shared" si="9"/>
-        <v>4.3782837127845885E-2</v>
+        <v>6.5674255691768824E-2</v>
       </c>
       <c r="H113">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I113">
         <f t="shared" si="11"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4418,15 +4422,15 @@
       </c>
       <c r="G114">
         <f t="shared" si="9"/>
-        <v>3.8284839203675348E-2</v>
+        <v>5.7427258805513019E-2</v>
       </c>
       <c r="H114">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I114">
         <f t="shared" si="11"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4453,15 +4457,15 @@
       </c>
       <c r="G115">
         <f t="shared" si="9"/>
-        <v>3.2819166393173609E-2</v>
+        <v>4.9228749589760423E-2</v>
       </c>
       <c r="H115">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I115">
         <f t="shared" si="11"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4488,15 +4492,15 @@
       </c>
       <c r="G116">
         <f t="shared" si="9"/>
-        <v>3.0111412225233364E-2</v>
+        <v>4.5167118337850046E-2</v>
       </c>
       <c r="H116">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I116">
         <f t="shared" si="11"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4523,15 +4527,15 @@
       </c>
       <c r="G117">
         <f t="shared" si="9"/>
-        <v>2.7419797093501508E-2</v>
+        <v>4.1129695640252262E-2</v>
       </c>
       <c r="H117">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I117">
         <f t="shared" si="11"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4558,15 +4562,15 @@
       </c>
       <c r="G118">
         <f t="shared" si="9"/>
-        <v>2.4746349913387779E-2</v>
+        <v>3.7119524870081667E-2</v>
       </c>
       <c r="H118">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I118">
         <f t="shared" si="11"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4593,15 +4597,15 @@
       </c>
       <c r="G119">
         <f t="shared" si="9"/>
-        <v>2.2128789555211331E-2</v>
+        <v>3.319318433281699E-2</v>
       </c>
       <c r="H119">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I119">
         <f t="shared" si="11"/>
-        <v>1.8518518518518521E-6</v>
+        <v>2.4074074074074076E-3</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4628,15 +4632,15 @@
       </c>
       <c r="G120">
         <f t="shared" si="9"/>
-        <v>1.9573302016050106E-2</v>
+        <v>2.935995302407516E-2</v>
       </c>
       <c r="H120">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I120">
         <f t="shared" si="11"/>
-        <v>2.2222222222222221E-6</v>
+        <v>2.4444444444444444E-3</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4663,15 +4667,15 @@
       </c>
       <c r="G121">
         <f t="shared" si="9"/>
-        <v>1.7158544955387784E-2</v>
+        <v>2.5737817433081678E-2</v>
       </c>
       <c r="H121">
         <f t="shared" si="10"/>
-        <v>2.6798874447273214E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I121">
         <f t="shared" si="11"/>
-        <v>2.7777777777777775E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4698,15 +4702,15 @@
       </c>
       <c r="G122">
         <f t="shared" si="9"/>
-        <v>6.2893081761006289E-2</v>
+        <v>9.4339622641509441E-2</v>
       </c>
       <c r="H122">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I122">
         <f t="shared" si="11"/>
-        <v>5.8479532163742688E-7</v>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4733,15 +4737,15 @@
       </c>
       <c r="G123">
         <f t="shared" si="9"/>
-        <v>5.9952038369304551E-2</v>
+        <v>8.9928057553956844E-2</v>
       </c>
       <c r="H123">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I123">
         <f t="shared" si="11"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4768,15 +4772,15 @@
       </c>
       <c r="G124">
         <f t="shared" si="9"/>
-        <v>5.4054054054054057E-2</v>
+        <v>8.1081081081081072E-2</v>
       </c>
       <c r="H124">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I124">
         <f t="shared" si="11"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4803,15 +4807,15 @@
       </c>
       <c r="G125">
         <f t="shared" si="9"/>
-        <v>4.8169556840077073E-2</v>
+        <v>7.2254335260115599E-2</v>
       </c>
       <c r="H125">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I125">
         <f t="shared" si="11"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4838,15 +4842,15 @@
       </c>
       <c r="G126">
         <f t="shared" si="9"/>
-        <v>4.2354934349851756E-2</v>
+        <v>6.353240152477764E-2</v>
       </c>
       <c r="H126">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I126">
         <f t="shared" si="11"/>
-        <v>9.2592592592592604E-7</v>
+        <v>2.3148148148148151E-3</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4873,15 +4877,15 @@
       </c>
       <c r="G127">
         <f t="shared" si="9"/>
-        <v>3.6576444769568402E-2</v>
+        <v>5.4864667154352592E-2</v>
       </c>
       <c r="H127">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I127">
         <f t="shared" si="11"/>
-        <v>1.111111111111111E-6</v>
+        <v>2.3333333333333335E-3</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4908,15 +4912,15 @@
       </c>
       <c r="G128">
         <f t="shared" si="9"/>
-        <v>3.3726812816188868E-2</v>
+        <v>5.0590219224283299E-2</v>
       </c>
       <c r="H128">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I128">
         <f t="shared" si="11"/>
-        <v>1.2345679012345681E-6</v>
+        <v>2.345679012345679E-3</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4943,15 +4947,15 @@
       </c>
       <c r="G129">
         <f t="shared" si="9"/>
-        <v>3.0911901081916538E-2</v>
+        <v>4.6367851622874809E-2</v>
       </c>
       <c r="H129">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I129">
         <f t="shared" si="11"/>
-        <v>1.3888888888888887E-6</v>
+        <v>2.3611111111111111E-3</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4978,15 +4982,15 @@
       </c>
       <c r="G130">
         <f t="shared" si="9"/>
-        <v>2.8153153153153147E-2</v>
+        <v>4.2229729729729729E-2</v>
       </c>
       <c r="H130">
         <f t="shared" si="10"/>
-        <v>2.8723251472066643E-4</v>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="I130">
         <f t="shared" si="11"/>
-        <v>1.5873015873015871E-6</v>
+        <v>2.3809523809523812E-3</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -5012,16 +5016,16 @@
         <v>10.526315789473685</v>
       </c>
       <c r="G131">
-        <f t="shared" ref="G131:G134" si="15">0.01*101325/D131*100</f>
-        <v>6.9589422407794019E-2</v>
+        <f t="shared" ref="G131:G134" si="15">0.015*101325/D131*100</f>
+        <v>0.10438413361169101</v>
       </c>
       <c r="H131">
-        <f t="shared" ref="H131:H134" si="16">0.001/E131*100</f>
-        <v>3.0945381401825781E-4</v>
+        <f t="shared" ref="H131:H134" si="16">0.001/B131*100</f>
+        <v>2E-3</v>
       </c>
       <c r="I131">
-        <f t="shared" ref="I131:I134" si="17">0.5*0.000000001*F131/(9*0.001)</f>
-        <v>5.8479532163742688E-7</v>
+        <f t="shared" ref="I131:I134" si="17">(0.2/9000+F131/(9*0.001)*0.5*0.000000001)*100</f>
+        <v>2.2807017543859647E-3</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -5048,15 +5052,15 @@
       </c>
       <c r="G132">
         <f t="shared" si="15"/>
-        <v>6.6445182724252497E-2</v>
+        <v>9.9667774086378724E-2</v>
       </c>
       <c r="H132">
         <f t="shared" si="16"/>
-        <v>3.0945381401825781E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="I132">
         <f t="shared" si="17"/>
-        <v>6.1728395061728406E-7</v>
+        <v>2.2839506172839504E-3</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -5083,15 +5087,15 @@
       </c>
       <c r="G133">
         <f t="shared" si="15"/>
-        <v>6.0168471720818295E-2</v>
+        <v>9.0252707581227443E-2</v>
       </c>
       <c r="H133">
         <f t="shared" si="16"/>
-        <v>3.0945381401825781E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="I133">
         <f t="shared" si="17"/>
-        <v>6.9444444444444437E-7</v>
+        <v>2.2916666666666667E-3</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -5118,15 +5122,15 @@
       </c>
       <c r="G134">
         <f t="shared" si="15"/>
-        <v>5.3937432578209273E-2</v>
+        <v>8.0906148867313926E-2</v>
       </c>
       <c r="H134">
         <f t="shared" si="16"/>
-        <v>3.0945381401825781E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="I134">
         <f t="shared" si="17"/>
-        <v>7.9365079365079355E-7</v>
+        <v>2.3015873015873019E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>